<commit_message>
chore(script): albertine gsheet wip
</commit_message>
<xml_diff>
--- a/script/python/albertine/ANIMATIONS 2025.xlsx
+++ b/script/python/albertine/ANIMATIONS 2025.xlsx
@@ -416,14 +416,14 @@
     <xf fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="14" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf fontId="2" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="14" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="2" fillId="5" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -947,13 +947,14 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="100" workbookViewId="0">
       <selection activeCell="J3" activeCellId="0" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="2" style="1" width="11.42578125"/>
+    <col min="1" max="1" style="1" width="11.42578125"/>
+    <col customWidth="1" min="2" max="2" style="1" width="29.140625"/>
     <col customWidth="1" min="3" max="3" style="1" width="47"/>
     <col customWidth="1" min="4" max="4" style="1" width="21.7109375"/>
     <col customWidth="1" min="5" max="5" style="1" width="31.5703125"/>
@@ -1011,7 +1012,7 @@
     </row>
     <row r="3" ht="42.75">
       <c r="A3" s="6"/>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C3" s="5" t="s">
@@ -1034,10 +1035,10 @@
       </c>
     </row>
     <row r="4" ht="28.5">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="7" t="s">
         <v>21</v>
       </c>
       <c r="C4" s="5" t="s">
@@ -1056,8 +1057,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" ht="42.75">
-      <c r="A5" s="8"/>
+    <row r="5" ht="28.5">
+      <c r="A5" s="9"/>
       <c r="B5" s="4" t="s">
         <v>27</v>
       </c>
@@ -1078,8 +1079,8 @@
       </c>
     </row>
     <row r="6" ht="28.5">
-      <c r="A6" s="8"/>
-      <c r="B6" s="9" t="s">
+      <c r="A6" s="9"/>
+      <c r="B6" s="4" t="s">
         <v>32</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -1099,7 +1100,7 @@
       </c>
     </row>
     <row r="7" ht="42.75">
-      <c r="A7" s="8"/>
+      <c r="A7" s="9"/>
       <c r="B7" s="1" t="s">
         <v>36</v>
       </c>
@@ -1123,8 +1124,8 @@
       </c>
     </row>
     <row r="8" ht="42.75">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9" t="s">
+      <c r="A8" s="9"/>
+      <c r="B8" s="4" t="s">
         <v>43</v>
       </c>
       <c r="C8" s="5" t="s">
@@ -1144,8 +1145,8 @@
       </c>
     </row>
     <row r="9" ht="42.75">
-      <c r="A9" s="8"/>
-      <c r="B9" s="4" t="s">
+      <c r="A9" s="9"/>
+      <c r="B9" s="7" t="s">
         <v>45</v>
       </c>
       <c r="C9" s="5" t="s">
@@ -1168,8 +1169,8 @@
       </c>
     </row>
     <row r="10" ht="28.5">
-      <c r="A10" s="8"/>
-      <c r="B10" s="4" t="s">
+      <c r="A10" s="9"/>
+      <c r="B10" s="7" t="s">
         <v>51</v>
       </c>
       <c r="C10" s="5" t="s">
@@ -1189,8 +1190,8 @@
       </c>
     </row>
     <row r="11" ht="28.5">
-      <c r="A11" s="8"/>
-      <c r="B11" s="9" t="s">
+      <c r="A11" s="9"/>
+      <c r="B11" s="4" t="s">
         <v>55</v>
       </c>
       <c r="C11" s="5" t="s">
@@ -1213,7 +1214,7 @@
       <c r="A12" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="7" t="s">
         <v>60</v>
       </c>
       <c r="C12" s="5" t="s">
@@ -1237,7 +1238,7 @@
     </row>
     <row r="13" ht="42.75">
       <c r="A13" s="11"/>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="7" t="s">
         <v>63</v>
       </c>
       <c r="C13" s="5" t="s">
@@ -1359,7 +1360,7 @@
     </row>
     <row r="18" ht="42.75">
       <c r="A18" s="13"/>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="7" t="s">
         <v>88</v>
       </c>
       <c r="C18" s="5" t="s">
@@ -1383,7 +1384,7 @@
     </row>
     <row r="19" ht="28.5">
       <c r="A19" s="13"/>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="7" t="s">
         <v>94</v>
       </c>
       <c r="C19" s="5" t="s">

</xml_diff>